<commit_message>
now with geiger summaries
</commit_message>
<xml_diff>
--- a/condor_approach/NormalizedRMSE.xlsx
+++ b/condor_approach/NormalizedRMSE.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">row.names</t>
   </si>
@@ -21,6 +21,9 @@
   </si>
   <si>
     <t xml:space="preserve">best.model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geiger.averaged</t>
   </si>
   <si>
     <t xml:space="preserve">sigma.sq</t>
@@ -83,11 +86,12 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C6" totalsRowCount="0" totalsRowShown="0">
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:D6" totalsRowCount="0" totalsRowShown="0">
+  <tableColumns count="4">
     <tableColumn id="1" name="row.names"/>
     <tableColumn id="2" name="model.averaged"/>
     <tableColumn id="3" name="best.model"/>
+    <tableColumn id="4" name="geiger.averaged"/>
   </tableColumns>
   <tableStyleInfo name="none" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -388,60 +392,74 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>0.463579361657651</v>
+        <v>0.464699131312926</v>
       </c>
       <c r="C2" t="n">
-        <v>0.493563402159026</v>
+        <v>0.490331077891466</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.59445809846249</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.511552245782057</v>
+        <v>0.515997903617863</v>
       </c>
       <c r="C3" t="n">
-        <v>0.524802383348079</v>
+        <v>0.524163591347172</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.683199800574798</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.580975653477715</v>
+        <v>0.65527111860267</v>
       </c>
       <c r="C4" t="n">
-        <v>0.738773869755208</v>
-      </c>
+        <v>0.802733037540415</v>
+      </c>
+      <c r="D4"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>1.98107512803569</v>
+        <v>1.88861055097863</v>
       </c>
       <c r="C5" t="n">
-        <v>2.2976944323937</v>
-      </c>
+        <v>2.24928758578876</v>
+      </c>
+      <c r="D5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.479400977325425</v>
+        <v>0.502708803448382</v>
       </c>
       <c r="C6" t="n">
-        <v>0.497798713984257</v>
+        <v>0.523339725627166</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4.25705506189245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
101 runs still going
</commit_message>
<xml_diff>
--- a/condor_approach/NormalizedRMSE.xlsx
+++ b/condor_approach/NormalizedRMSE.xlsx
@@ -415,19 +415,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>0.464699131312926</v>
+        <v>0.453262894143333</v>
       </c>
       <c r="C2" t="n">
-        <v>0.490331077891466</v>
+        <v>0.464946826018322</v>
       </c>
       <c r="D2" t="n">
-        <v>1.20811647181057</v>
+        <v>1.34141229309264</v>
       </c>
       <c r="E2" t="n">
-        <v>0.536607312656955</v>
+        <v>0.465606710193433</v>
       </c>
       <c r="F2" t="n">
-        <v>0.576714133171311</v>
+        <v>1.80132753706707</v>
       </c>
     </row>
     <row r="3">
@@ -435,19 +435,19 @@
         <v>7</v>
       </c>
       <c r="B3" t="n">
-        <v>0.515997903617863</v>
+        <v>0.536640908522899</v>
       </c>
       <c r="C3" t="n">
-        <v>0.524163591347172</v>
+        <v>0.545583290549336</v>
       </c>
       <c r="D3" t="n">
-        <v>0.682475651475411</v>
+        <v>0.870076413594506</v>
       </c>
       <c r="E3" t="n">
-        <v>0.458928763872188</v>
+        <v>0.392518932226337</v>
       </c>
       <c r="F3" t="n">
-        <v>0.459687137760183</v>
+        <v>0.374672849089424</v>
       </c>
     </row>
     <row r="4">
@@ -455,14 +455,14 @@
         <v>8</v>
       </c>
       <c r="B4" t="n">
-        <v>0.65527111860267</v>
+        <v>0.488556234623904</v>
       </c>
       <c r="C4" t="n">
-        <v>0.802733037540415</v>
+        <v>0.597115893972384</v>
       </c>
       <c r="D4"/>
       <c r="E4" t="n">
-        <v>0.302167621597189</v>
+        <v>0.243154295480897</v>
       </c>
       <c r="F4"/>
     </row>
@@ -471,10 +471,10 @@
         <v>9</v>
       </c>
       <c r="B5" t="n">
-        <v>1.88861055097863</v>
+        <v>1.62749589944488</v>
       </c>
       <c r="C5" t="n">
-        <v>2.24928758578876</v>
+        <v>1.77114502143414</v>
       </c>
       <c r="D5"/>
       <c r="E5"/>
@@ -485,19 +485,19 @@
         <v>10</v>
       </c>
       <c r="B6" t="n">
-        <v>0.502708803448382</v>
+        <v>0.522569588062163</v>
       </c>
       <c r="C6" t="n">
-        <v>0.523339725627166</v>
+        <v>0.534021610917451</v>
       </c>
       <c r="D6" t="n">
-        <v>4.41980184309945</v>
+        <v>4.52652963238878</v>
       </c>
       <c r="E6" t="n">
-        <v>0.527231827278011</v>
+        <v>0.534752274100427</v>
       </c>
       <c r="F6" t="n">
-        <v>4.3070017392519</v>
+        <v>4.39407843884091</v>
       </c>
     </row>
   </sheetData>

</xml_diff>